<commit_message>
Final draft for review
</commit_message>
<xml_diff>
--- a/Data_Sources/Occupancy_Ideas.xlsx
+++ b/Data_Sources/Occupancy_Ideas.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/Travel_Co_Analysis/Notebooks_Data_Generation/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stuartgow/GitHub/Travel_Co_Analysis/Data_Sources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A136B345-3BC5-EC43-8BEF-84AFD64F1908}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{500E1288-2377-3040-8D1F-980DD465F52F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="580" yWindow="780" windowWidth="35260" windowHeight="22780" xr2:uid="{04353748-68C1-8048-B2FA-FC1ED23A3AD3}"/>
+    <workbookView xWindow="4880" yWindow="780" windowWidth="35260" windowHeight="22780" xr2:uid="{04353748-68C1-8048-B2FA-FC1ED23A3AD3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -91,7 +91,7 @@
     <numFmt numFmtId="164" formatCode="0.0%"/>
     <numFmt numFmtId="165" formatCode="&quot;£&quot;#,##0"/>
   </numFmts>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -99,8 +99,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,8 +144,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -146,11 +159,91 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -173,25 +266,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,21 +657,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25BB408F-32E1-804F-95A7-FB96F8CFF522}">
-  <dimension ref="A1:O33"/>
+  <dimension ref="A1:M33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+      <selection activeCell="O12" sqref="O12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="1"/>
-    <col min="6" max="6" width="1.83203125" customWidth="1"/>
-    <col min="11" max="11" width="2" customWidth="1"/>
+    <col min="1" max="1" width="11.6640625" style="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A1" s="17" t="s">
+    <row r="1" spans="1:13" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
@@ -549,1521 +678,1520 @@
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
-      <c r="G1" s="14" t="s">
+      <c r="F1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="14"/>
-      <c r="I1" s="14"/>
-      <c r="J1" s="14"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="15" t="s">
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
+      <c r="I1" s="15"/>
+      <c r="J1" s="16" t="s">
         <v>13</v>
       </c>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="15"/>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="B2" s="13" t="s">
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="18" t="s">
+      <c r="C2" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="19" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="13" t="s">
+      <c r="F2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="G2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="J2" s="13" t="s">
+      <c r="H2" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="I2" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="13"/>
-      <c r="L2" s="12" t="s">
+      <c r="J2" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="M2" s="12" t="s">
+      <c r="K2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="12" t="s">
+      <c r="L2" s="21" t="s">
         <v>5</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="M2" s="22" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="23">
         <v>45658</v>
       </c>
-      <c r="B3">
-        <v>30</v>
-      </c>
-      <c r="C3" s="16">
-        <v>150</v>
-      </c>
-      <c r="D3">
-        <v>10</v>
-      </c>
-      <c r="E3" s="5">
+      <c r="B3" s="24">
+        <v>30</v>
+      </c>
+      <c r="C3" s="25">
+        <v>150</v>
+      </c>
+      <c r="D3" s="24">
+        <v>10</v>
+      </c>
+      <c r="E3" s="26">
         <f>D3/B3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G3">
-        <v>10</v>
-      </c>
-      <c r="H3" s="16">
-        <v>225</v>
-      </c>
-      <c r="I3">
+      <c r="F3" s="27">
+        <v>10</v>
+      </c>
+      <c r="G3" s="28">
+        <v>225</v>
+      </c>
+      <c r="H3" s="27">
         <v>5</v>
       </c>
-      <c r="J3" s="5">
-        <f>I3/G3</f>
+      <c r="I3" s="29">
+        <f>H3/F3</f>
         <v>0.5</v>
       </c>
-      <c r="L3" s="5">
-        <f>(D3+I3)/(B3+G3)</f>
+      <c r="J3" s="30">
+        <f>(D3+H3)/(B3+F3)</f>
         <v>0.375</v>
       </c>
-      <c r="M3" s="16">
-        <f>(C3*D3)+(H3*I3)</f>
+      <c r="K3" s="31">
+        <f>(C3*D3)+(G3*H3)</f>
         <v>2625</v>
       </c>
-      <c r="N3" s="16">
-        <f>M3/(D3+I3)</f>
+      <c r="L3" s="31">
+        <f>K3/(D3+H3)</f>
         <v>175</v>
       </c>
-      <c r="O3" s="16">
-        <f>L3*N3</f>
+      <c r="M3" s="32">
+        <f>J3*L3</f>
         <v>65.625</v>
       </c>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A4" s="2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A4" s="23">
         <v>45659</v>
       </c>
-      <c r="B4">
-        <v>30</v>
-      </c>
-      <c r="C4" s="16">
-        <v>150</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="24">
+        <v>30</v>
+      </c>
+      <c r="C4" s="25">
+        <v>150</v>
+      </c>
+      <c r="D4" s="24">
         <v>15</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="26">
         <f t="shared" ref="E4:E33" si="0">D4/B4</f>
         <v>0.5</v>
       </c>
-      <c r="G4">
-        <v>10</v>
-      </c>
-      <c r="H4" s="16">
-        <v>225</v>
-      </c>
-      <c r="I4">
+      <c r="F4" s="27">
+        <v>10</v>
+      </c>
+      <c r="G4" s="28">
+        <v>225</v>
+      </c>
+      <c r="H4" s="27">
         <v>5</v>
       </c>
-      <c r="J4" s="5">
-        <f t="shared" ref="J4:J33" si="1">I4/G4</f>
+      <c r="I4" s="29">
+        <f t="shared" ref="I4:I33" si="1">H4/F4</f>
         <v>0.5</v>
       </c>
-      <c r="L4" s="5">
-        <f>(D4+I4)/(B4+G4)</f>
+      <c r="J4" s="30">
+        <f>(D4+H4)/(B4+F4)</f>
         <v>0.5</v>
       </c>
-      <c r="M4" s="16">
-        <f>(C4*D4)+(H4*I4)</f>
+      <c r="K4" s="31">
+        <f>(C4*D4)+(G4*H4)</f>
         <v>3375</v>
       </c>
-      <c r="N4" s="16">
-        <f>M4/(D4+I4)</f>
+      <c r="L4" s="31">
+        <f>K4/(D4+H4)</f>
         <v>168.75</v>
       </c>
-      <c r="O4" s="16">
-        <f t="shared" ref="O4:O33" si="2">L4*N4</f>
+      <c r="M4" s="32">
+        <f t="shared" ref="M4:M33" si="2">J4*L4</f>
         <v>84.375</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A5" s="2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A5" s="23">
         <v>45660</v>
       </c>
-      <c r="B5">
-        <v>30</v>
-      </c>
-      <c r="C5" s="16">
-        <v>150</v>
-      </c>
-      <c r="D5">
+      <c r="B5" s="24">
+        <v>30</v>
+      </c>
+      <c r="C5" s="25">
+        <v>150</v>
+      </c>
+      <c r="D5" s="24">
         <v>21</v>
       </c>
-      <c r="E5" s="5">
+      <c r="E5" s="26">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G5">
-        <v>10</v>
-      </c>
-      <c r="H5" s="16">
-        <v>225</v>
-      </c>
-      <c r="I5">
+      <c r="F5" s="27">
+        <v>10</v>
+      </c>
+      <c r="G5" s="28">
+        <v>225</v>
+      </c>
+      <c r="H5" s="27">
         <v>2</v>
       </c>
-      <c r="J5" s="5">
+      <c r="I5" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L5" s="5">
-        <f>(D5+I5)/(B5+G5)</f>
+      <c r="J5" s="30">
+        <f>(D5+H5)/(B5+F5)</f>
         <v>0.57499999999999996</v>
       </c>
-      <c r="M5" s="16">
-        <f>(C5*D5)+(H5*I5)</f>
+      <c r="K5" s="31">
+        <f>(C5*D5)+(G5*H5)</f>
         <v>3600</v>
       </c>
-      <c r="N5" s="16">
-        <f>M5/(D5+I5)</f>
+      <c r="L5" s="31">
+        <f>K5/(D5+H5)</f>
         <v>156.52173913043478</v>
       </c>
-      <c r="O5" s="16">
+      <c r="M5" s="32">
         <f t="shared" si="2"/>
         <v>89.999999999999986</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A6" s="2">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="23">
         <v>45661</v>
       </c>
-      <c r="B6">
-        <v>30</v>
-      </c>
-      <c r="C6" s="16">
-        <v>150</v>
-      </c>
-      <c r="D6">
+      <c r="B6" s="24">
+        <v>30</v>
+      </c>
+      <c r="C6" s="25">
+        <v>150</v>
+      </c>
+      <c r="D6" s="24">
         <v>5</v>
       </c>
-      <c r="E6" s="5">
+      <c r="E6" s="26">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G6">
-        <v>10</v>
-      </c>
-      <c r="H6" s="16">
-        <v>225</v>
-      </c>
-      <c r="I6">
+      <c r="F6" s="27">
+        <v>10</v>
+      </c>
+      <c r="G6" s="28">
+        <v>225</v>
+      </c>
+      <c r="H6" s="27">
         <v>0</v>
       </c>
-      <c r="J6" s="5">
+      <c r="I6" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L6" s="5">
-        <f>(D6+I6)/(B6+G6)</f>
+      <c r="J6" s="30">
+        <f>(D6+H6)/(B6+F6)</f>
         <v>0.125</v>
       </c>
-      <c r="M6" s="16">
-        <f>(C6*D6)+(H6*I6)</f>
+      <c r="K6" s="31">
+        <f>(C6*D6)+(G6*H6)</f>
         <v>750</v>
       </c>
-      <c r="N6" s="16">
-        <f>M6/(D6+I6)</f>
-        <v>150</v>
-      </c>
-      <c r="O6" s="16">
+      <c r="L6" s="31">
+        <f>K6/(D6+H6)</f>
+        <v>150</v>
+      </c>
+      <c r="M6" s="32">
         <f t="shared" si="2"/>
         <v>18.75</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A7" s="2">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="23">
         <v>45662</v>
       </c>
-      <c r="B7">
-        <v>30</v>
-      </c>
-      <c r="C7" s="16">
-        <v>150</v>
-      </c>
-      <c r="D7">
-        <v>30</v>
-      </c>
-      <c r="E7" s="5">
+      <c r="B7" s="24">
+        <v>30</v>
+      </c>
+      <c r="C7" s="25">
+        <v>150</v>
+      </c>
+      <c r="D7" s="24">
+        <v>30</v>
+      </c>
+      <c r="E7" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G7">
-        <v>10</v>
-      </c>
-      <c r="H7" s="16">
-        <v>225</v>
-      </c>
-      <c r="I7">
+      <c r="F7" s="27">
+        <v>10</v>
+      </c>
+      <c r="G7" s="28">
+        <v>225</v>
+      </c>
+      <c r="H7" s="27">
         <v>3</v>
       </c>
-      <c r="J7" s="5">
+      <c r="I7" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L7" s="5">
-        <f>(D7+I7)/(B7+G7)</f>
+      <c r="J7" s="30">
+        <f>(D7+H7)/(B7+F7)</f>
         <v>0.82499999999999996</v>
       </c>
-      <c r="M7" s="16">
-        <f>(C7*D7)+(H7*I7)</f>
+      <c r="K7" s="31">
+        <f>(C7*D7)+(G7*H7)</f>
         <v>5175</v>
       </c>
-      <c r="N7" s="16">
-        <f>M7/(D7+I7)</f>
+      <c r="L7" s="31">
+        <f>K7/(D7+H7)</f>
         <v>156.81818181818181</v>
       </c>
-      <c r="O7" s="16">
+      <c r="M7" s="32">
         <f t="shared" si="2"/>
         <v>129.375</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A8" s="2">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="23">
         <v>45663</v>
       </c>
-      <c r="B8">
-        <v>30</v>
-      </c>
-      <c r="C8" s="16">
-        <v>150</v>
-      </c>
-      <c r="D8">
-        <v>30</v>
-      </c>
-      <c r="E8" s="5">
+      <c r="B8" s="24">
+        <v>30</v>
+      </c>
+      <c r="C8" s="25">
+        <v>150</v>
+      </c>
+      <c r="D8" s="24">
+        <v>30</v>
+      </c>
+      <c r="E8" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G8">
-        <v>10</v>
-      </c>
-      <c r="H8" s="16">
-        <v>225</v>
-      </c>
-      <c r="I8">
+      <c r="F8" s="27">
+        <v>10</v>
+      </c>
+      <c r="G8" s="28">
+        <v>225</v>
+      </c>
+      <c r="H8" s="27">
         <v>3</v>
       </c>
-      <c r="J8" s="5">
+      <c r="I8" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L8" s="5">
-        <f>(D8+I8)/(B8+G8)</f>
+      <c r="J8" s="30">
+        <f>(D8+H8)/(B8+F8)</f>
         <v>0.82499999999999996</v>
       </c>
-      <c r="M8" s="16">
-        <f>(C8*D8)+(H8*I8)</f>
+      <c r="K8" s="31">
+        <f>(C8*D8)+(G8*H8)</f>
         <v>5175</v>
       </c>
-      <c r="N8" s="16">
-        <f>M8/(D8+I8)</f>
+      <c r="L8" s="31">
+        <f>K8/(D8+H8)</f>
         <v>156.81818181818181</v>
       </c>
-      <c r="O8" s="16">
+      <c r="M8" s="32">
         <f t="shared" si="2"/>
         <v>129.375</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A9" s="2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A9" s="23">
         <v>45664</v>
       </c>
-      <c r="B9">
-        <v>30</v>
-      </c>
-      <c r="C9" s="16">
-        <v>150</v>
-      </c>
-      <c r="D9">
+      <c r="B9" s="24">
+        <v>30</v>
+      </c>
+      <c r="C9" s="25">
+        <v>150</v>
+      </c>
+      <c r="D9" s="24">
         <v>15</v>
       </c>
-      <c r="E9" s="5">
+      <c r="E9" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G9">
-        <v>10</v>
-      </c>
-      <c r="H9" s="16">
-        <v>225</v>
-      </c>
-      <c r="I9">
+      <c r="F9" s="27">
+        <v>10</v>
+      </c>
+      <c r="G9" s="28">
+        <v>225</v>
+      </c>
+      <c r="H9" s="27">
         <v>8</v>
       </c>
-      <c r="J9" s="5">
+      <c r="I9" s="29">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="L9" s="5">
-        <f>(D9+I9)/(B9+G9)</f>
+      <c r="J9" s="30">
+        <f>(D9+H9)/(B9+F9)</f>
         <v>0.57499999999999996</v>
       </c>
-      <c r="M9" s="16">
-        <f>(C9*D9)+(H9*I9)</f>
+      <c r="K9" s="31">
+        <f>(C9*D9)+(G9*H9)</f>
         <v>4050</v>
       </c>
-      <c r="N9" s="16">
-        <f>M9/(D9+I9)</f>
+      <c r="L9" s="31">
+        <f>K9/(D9+H9)</f>
         <v>176.08695652173913</v>
       </c>
-      <c r="O9" s="16">
+      <c r="M9" s="32">
         <f t="shared" si="2"/>
         <v>101.24999999999999</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A10" s="23">
         <v>45665</v>
       </c>
-      <c r="B10">
-        <v>30</v>
-      </c>
-      <c r="C10" s="16">
-        <v>150</v>
-      </c>
-      <c r="D10">
-        <v>10</v>
-      </c>
-      <c r="E10" s="5">
+      <c r="B10" s="24">
+        <v>30</v>
+      </c>
+      <c r="C10" s="25">
+        <v>150</v>
+      </c>
+      <c r="D10" s="24">
+        <v>10</v>
+      </c>
+      <c r="E10" s="26">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G10">
-        <v>10</v>
-      </c>
-      <c r="H10" s="16">
-        <v>225</v>
-      </c>
-      <c r="I10">
+      <c r="F10" s="27">
+        <v>10</v>
+      </c>
+      <c r="G10" s="28">
+        <v>225</v>
+      </c>
+      <c r="H10" s="27">
         <v>9</v>
       </c>
-      <c r="J10" s="5">
+      <c r="I10" s="29">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="L10" s="5">
-        <f>(D10+I10)/(B10+G10)</f>
+      <c r="J10" s="30">
+        <f>(D10+H10)/(B10+F10)</f>
         <v>0.47499999999999998</v>
       </c>
-      <c r="M10" s="16">
-        <f>(C10*D10)+(H10*I10)</f>
+      <c r="K10" s="31">
+        <f>(C10*D10)+(G10*H10)</f>
         <v>3525</v>
       </c>
-      <c r="N10" s="16">
-        <f>M10/(D10+I10)</f>
+      <c r="L10" s="31">
+        <f>K10/(D10+H10)</f>
         <v>185.52631578947367</v>
       </c>
-      <c r="O10" s="16">
+      <c r="M10" s="32">
         <f t="shared" si="2"/>
         <v>88.124999999999986</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A11" s="23">
         <v>45666</v>
       </c>
-      <c r="B11">
-        <v>30</v>
-      </c>
-      <c r="C11" s="16">
-        <v>150</v>
-      </c>
-      <c r="D11">
+      <c r="B11" s="24">
+        <v>30</v>
+      </c>
+      <c r="C11" s="25">
+        <v>150</v>
+      </c>
+      <c r="D11" s="24">
         <v>15</v>
       </c>
-      <c r="E11" s="5">
+      <c r="E11" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G11">
-        <v>10</v>
-      </c>
-      <c r="H11" s="16">
-        <v>225</v>
-      </c>
-      <c r="I11">
-        <v>10</v>
-      </c>
-      <c r="J11" s="5">
+      <c r="F11" s="27">
+        <v>10</v>
+      </c>
+      <c r="G11" s="28">
+        <v>225</v>
+      </c>
+      <c r="H11" s="27">
+        <v>10</v>
+      </c>
+      <c r="I11" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L11" s="5">
-        <f>(D11+I11)/(B11+G11)</f>
+      <c r="J11" s="30">
+        <f>(D11+H11)/(B11+F11)</f>
         <v>0.625</v>
       </c>
-      <c r="M11" s="16">
-        <f>(C11*D11)+(H11*I11)</f>
+      <c r="K11" s="31">
+        <f>(C11*D11)+(G11*H11)</f>
         <v>4500</v>
       </c>
-      <c r="N11" s="16">
-        <f>M11/(D11+I11)</f>
+      <c r="L11" s="31">
+        <f>K11/(D11+H11)</f>
         <v>180</v>
       </c>
-      <c r="O11" s="16">
+      <c r="M11" s="32">
         <f t="shared" si="2"/>
         <v>112.5</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A12" s="2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A12" s="23">
         <v>45667</v>
       </c>
-      <c r="B12">
-        <v>30</v>
-      </c>
-      <c r="C12" s="16">
-        <v>150</v>
-      </c>
-      <c r="D12">
+      <c r="B12" s="24">
+        <v>30</v>
+      </c>
+      <c r="C12" s="25">
+        <v>150</v>
+      </c>
+      <c r="D12" s="24">
         <v>21</v>
       </c>
-      <c r="E12" s="5">
+      <c r="E12" s="26">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G12">
-        <v>10</v>
-      </c>
-      <c r="H12" s="16">
-        <v>225</v>
-      </c>
-      <c r="I12">
+      <c r="F12" s="27">
+        <v>10</v>
+      </c>
+      <c r="G12" s="28">
+        <v>225</v>
+      </c>
+      <c r="H12" s="27">
         <v>2</v>
       </c>
-      <c r="J12" s="5">
+      <c r="I12" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L12" s="5">
-        <f>(D12+I12)/(B12+G12)</f>
+      <c r="J12" s="30">
+        <f>(D12+H12)/(B12+F12)</f>
         <v>0.57499999999999996</v>
       </c>
-      <c r="M12" s="16">
-        <f>(C12*D12)+(H12*I12)</f>
+      <c r="K12" s="31">
+        <f>(C12*D12)+(G12*H12)</f>
         <v>3600</v>
       </c>
-      <c r="N12" s="16">
-        <f>M12/(D12+I12)</f>
+      <c r="L12" s="31">
+        <f>K12/(D12+H12)</f>
         <v>156.52173913043478</v>
       </c>
-      <c r="O12" s="16">
+      <c r="M12" s="32">
         <f t="shared" si="2"/>
         <v>89.999999999999986</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A13" s="2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A13" s="23">
         <v>45668</v>
       </c>
-      <c r="B13">
-        <v>30</v>
-      </c>
-      <c r="C13" s="16">
-        <v>150</v>
-      </c>
-      <c r="D13">
+      <c r="B13" s="24">
+        <v>30</v>
+      </c>
+      <c r="C13" s="25">
+        <v>150</v>
+      </c>
+      <c r="D13" s="24">
         <v>5</v>
       </c>
-      <c r="E13" s="5">
+      <c r="E13" s="26">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G13">
-        <v>10</v>
-      </c>
-      <c r="H13" s="16">
-        <v>225</v>
-      </c>
-      <c r="I13">
+      <c r="F13" s="27">
+        <v>10</v>
+      </c>
+      <c r="G13" s="28">
+        <v>225</v>
+      </c>
+      <c r="H13" s="27">
         <v>4</v>
       </c>
-      <c r="J13" s="5">
+      <c r="I13" s="29">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="L13" s="5">
-        <f>(D13+I13)/(B13+G13)</f>
+      <c r="J13" s="30">
+        <f>(D13+H13)/(B13+F13)</f>
         <v>0.22500000000000001</v>
       </c>
-      <c r="M13" s="16">
-        <f>(C13*D13)+(H13*I13)</f>
+      <c r="K13" s="31">
+        <f>(C13*D13)+(G13*H13)</f>
         <v>1650</v>
       </c>
-      <c r="N13" s="16">
-        <f>M13/(D13+I13)</f>
+      <c r="L13" s="31">
+        <f>K13/(D13+H13)</f>
         <v>183.33333333333334</v>
       </c>
-      <c r="O13" s="16">
+      <c r="M13" s="32">
         <f t="shared" si="2"/>
         <v>41.25</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A14" s="2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A14" s="23">
         <v>45669</v>
       </c>
-      <c r="B14">
-        <v>30</v>
-      </c>
-      <c r="C14" s="16">
-        <v>150</v>
-      </c>
-      <c r="D14">
-        <v>30</v>
-      </c>
-      <c r="E14" s="5">
+      <c r="B14" s="24">
+        <v>30</v>
+      </c>
+      <c r="C14" s="25">
+        <v>150</v>
+      </c>
+      <c r="D14" s="24">
+        <v>30</v>
+      </c>
+      <c r="E14" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G14">
-        <v>10</v>
-      </c>
-      <c r="H14" s="16">
-        <v>225</v>
-      </c>
-      <c r="I14">
-        <v>10</v>
-      </c>
-      <c r="J14" s="5">
+      <c r="F14" s="27">
+        <v>10</v>
+      </c>
+      <c r="G14" s="28">
+        <v>225</v>
+      </c>
+      <c r="H14" s="27">
+        <v>10</v>
+      </c>
+      <c r="I14" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L14" s="5">
-        <f>(D14+I14)/(B14+G14)</f>
+      <c r="J14" s="30">
+        <f>(D14+H14)/(B14+F14)</f>
         <v>1</v>
       </c>
-      <c r="M14" s="16">
-        <f>(C14*D14)+(H14*I14)</f>
+      <c r="K14" s="31">
+        <f>(C14*D14)+(G14*H14)</f>
         <v>6750</v>
       </c>
-      <c r="N14" s="16">
-        <f>M14/(D14+I14)</f>
+      <c r="L14" s="31">
+        <f>K14/(D14+H14)</f>
         <v>168.75</v>
       </c>
-      <c r="O14" s="16">
+      <c r="M14" s="32">
         <f t="shared" si="2"/>
         <v>168.75</v>
       </c>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A15" s="2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A15" s="23">
         <v>45670</v>
       </c>
-      <c r="B15">
-        <v>30</v>
-      </c>
-      <c r="C15" s="16">
-        <v>150</v>
-      </c>
-      <c r="D15">
-        <v>30</v>
-      </c>
-      <c r="E15" s="5">
+      <c r="B15" s="24">
+        <v>30</v>
+      </c>
+      <c r="C15" s="25">
+        <v>150</v>
+      </c>
+      <c r="D15" s="24">
+        <v>30</v>
+      </c>
+      <c r="E15" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G15">
-        <v>10</v>
-      </c>
-      <c r="H15" s="16">
-        <v>225</v>
-      </c>
-      <c r="I15">
-        <v>10</v>
-      </c>
-      <c r="J15" s="5">
+      <c r="F15" s="27">
+        <v>10</v>
+      </c>
+      <c r="G15" s="28">
+        <v>225</v>
+      </c>
+      <c r="H15" s="27">
+        <v>10</v>
+      </c>
+      <c r="I15" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L15" s="5">
-        <f>(D15+I15)/(B15+G15)</f>
+      <c r="J15" s="30">
+        <f>(D15+H15)/(B15+F15)</f>
         <v>1</v>
       </c>
-      <c r="M15" s="16">
-        <f>(C15*D15)+(H15*I15)</f>
+      <c r="K15" s="31">
+        <f>(C15*D15)+(G15*H15)</f>
         <v>6750</v>
       </c>
-      <c r="N15" s="16">
-        <f>M15/(D15+I15)</f>
+      <c r="L15" s="31">
+        <f>K15/(D15+H15)</f>
         <v>168.75</v>
       </c>
-      <c r="O15" s="16">
+      <c r="M15" s="32">
         <f t="shared" si="2"/>
         <v>168.75</v>
       </c>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A16" s="2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A16" s="23">
         <v>45671</v>
       </c>
-      <c r="B16">
-        <v>30</v>
-      </c>
-      <c r="C16" s="16">
-        <v>150</v>
-      </c>
-      <c r="D16">
+      <c r="B16" s="24">
+        <v>30</v>
+      </c>
+      <c r="C16" s="25">
+        <v>150</v>
+      </c>
+      <c r="D16" s="24">
         <v>15</v>
       </c>
-      <c r="E16" s="5">
+      <c r="E16" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G16">
-        <v>10</v>
-      </c>
-      <c r="H16" s="16">
-        <v>225</v>
-      </c>
-      <c r="I16">
+      <c r="F16" s="27">
+        <v>10</v>
+      </c>
+      <c r="G16" s="28">
+        <v>225</v>
+      </c>
+      <c r="H16" s="27">
         <v>2</v>
       </c>
-      <c r="J16" s="5">
+      <c r="I16" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L16" s="5">
-        <f>(D16+I16)/(B16+G16)</f>
+      <c r="J16" s="30">
+        <f>(D16+H16)/(B16+F16)</f>
         <v>0.42499999999999999</v>
       </c>
-      <c r="M16" s="16">
-        <f>(C16*D16)+(H16*I16)</f>
+      <c r="K16" s="31">
+        <f>(C16*D16)+(G16*H16)</f>
         <v>2700</v>
       </c>
-      <c r="N16" s="16">
-        <f>M16/(D16+I16)</f>
+      <c r="L16" s="31">
+        <f>K16/(D16+H16)</f>
         <v>158.8235294117647</v>
       </c>
-      <c r="O16" s="16">
+      <c r="M16" s="32">
         <f t="shared" si="2"/>
         <v>67.5</v>
       </c>
     </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A17" s="2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A17" s="23">
         <v>45672</v>
       </c>
-      <c r="B17">
-        <v>30</v>
-      </c>
-      <c r="C17" s="16">
-        <v>150</v>
-      </c>
-      <c r="D17">
-        <v>10</v>
-      </c>
-      <c r="E17" s="5">
+      <c r="B17" s="24">
+        <v>30</v>
+      </c>
+      <c r="C17" s="25">
+        <v>150</v>
+      </c>
+      <c r="D17" s="24">
+        <v>10</v>
+      </c>
+      <c r="E17" s="26">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G17">
-        <v>10</v>
-      </c>
-      <c r="H17" s="16">
-        <v>225</v>
-      </c>
-      <c r="I17">
+      <c r="F17" s="27">
+        <v>10</v>
+      </c>
+      <c r="G17" s="28">
+        <v>225</v>
+      </c>
+      <c r="H17" s="27">
         <v>0</v>
       </c>
-      <c r="J17" s="5">
+      <c r="I17" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L17" s="5">
-        <f>(D17+I17)/(B17+G17)</f>
+      <c r="J17" s="30">
+        <f>(D17+H17)/(B17+F17)</f>
         <v>0.25</v>
       </c>
-      <c r="M17" s="16">
-        <f>(C17*D17)+(H17*I17)</f>
+      <c r="K17" s="31">
+        <f>(C17*D17)+(G17*H17)</f>
         <v>1500</v>
       </c>
-      <c r="N17" s="16">
-        <f>M17/(D17+I17)</f>
-        <v>150</v>
-      </c>
-      <c r="O17" s="16">
+      <c r="L17" s="31">
+        <f>K17/(D17+H17)</f>
+        <v>150</v>
+      </c>
+      <c r="M17" s="32">
         <f t="shared" si="2"/>
         <v>37.5</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A18" s="23">
         <v>45673</v>
       </c>
-      <c r="B18">
-        <v>30</v>
-      </c>
-      <c r="C18" s="16">
-        <v>150</v>
-      </c>
-      <c r="D18">
+      <c r="B18" s="24">
+        <v>30</v>
+      </c>
+      <c r="C18" s="25">
+        <v>150</v>
+      </c>
+      <c r="D18" s="24">
         <v>15</v>
       </c>
-      <c r="E18" s="5">
+      <c r="E18" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G18">
-        <v>10</v>
-      </c>
-      <c r="H18" s="16">
-        <v>225</v>
-      </c>
-      <c r="I18">
+      <c r="F18" s="27">
+        <v>10</v>
+      </c>
+      <c r="G18" s="28">
+        <v>225</v>
+      </c>
+      <c r="H18" s="27">
         <v>3</v>
       </c>
-      <c r="J18" s="5">
+      <c r="I18" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L18" s="5">
-        <f>(D18+I18)/(B18+G18)</f>
+      <c r="J18" s="30">
+        <f>(D18+H18)/(B18+F18)</f>
         <v>0.45</v>
       </c>
-      <c r="M18" s="16">
-        <f>(C18*D18)+(H18*I18)</f>
+      <c r="K18" s="31">
+        <f>(C18*D18)+(G18*H18)</f>
         <v>2925</v>
       </c>
-      <c r="N18" s="16">
-        <f>M18/(D18+I18)</f>
+      <c r="L18" s="31">
+        <f>K18/(D18+H18)</f>
         <v>162.5</v>
       </c>
-      <c r="O18" s="16">
+      <c r="M18" s="32">
         <f t="shared" si="2"/>
         <v>73.125</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A19" s="23">
         <v>45674</v>
       </c>
-      <c r="B19">
-        <v>30</v>
-      </c>
-      <c r="C19" s="16">
-        <v>150</v>
-      </c>
-      <c r="D19">
+      <c r="B19" s="24">
+        <v>30</v>
+      </c>
+      <c r="C19" s="25">
+        <v>150</v>
+      </c>
+      <c r="D19" s="24">
         <v>21</v>
       </c>
-      <c r="E19" s="5">
+      <c r="E19" s="26">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G19">
-        <v>10</v>
-      </c>
-      <c r="H19" s="16">
-        <v>225</v>
-      </c>
-      <c r="I19">
+      <c r="F19" s="27">
+        <v>10</v>
+      </c>
+      <c r="G19" s="28">
+        <v>225</v>
+      </c>
+      <c r="H19" s="27">
         <v>3</v>
       </c>
-      <c r="J19" s="5">
+      <c r="I19" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L19" s="5">
-        <f>(D19+I19)/(B19+G19)</f>
+      <c r="J19" s="30">
+        <f>(D19+H19)/(B19+F19)</f>
         <v>0.6</v>
       </c>
-      <c r="M19" s="16">
-        <f>(C19*D19)+(H19*I19)</f>
+      <c r="K19" s="31">
+        <f>(C19*D19)+(G19*H19)</f>
         <v>3825</v>
       </c>
-      <c r="N19" s="16">
-        <f>M19/(D19+I19)</f>
+      <c r="L19" s="31">
+        <f>K19/(D19+H19)</f>
         <v>159.375</v>
       </c>
-      <c r="O19" s="16">
+      <c r="M19" s="32">
         <f t="shared" si="2"/>
         <v>95.625</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A20" s="23">
         <v>45675</v>
       </c>
-      <c r="B20">
-        <v>30</v>
-      </c>
-      <c r="C20" s="16">
-        <v>150</v>
-      </c>
-      <c r="D20">
+      <c r="B20" s="24">
+        <v>30</v>
+      </c>
+      <c r="C20" s="25">
+        <v>150</v>
+      </c>
+      <c r="D20" s="24">
         <v>5</v>
       </c>
-      <c r="E20" s="5">
+      <c r="E20" s="26">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G20">
-        <v>10</v>
-      </c>
-      <c r="H20" s="16">
-        <v>225</v>
-      </c>
-      <c r="I20">
+      <c r="F20" s="27">
+        <v>10</v>
+      </c>
+      <c r="G20" s="28">
+        <v>225</v>
+      </c>
+      <c r="H20" s="27">
         <v>8</v>
       </c>
-      <c r="J20" s="5">
+      <c r="I20" s="29">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="L20" s="5">
-        <f>(D20+I20)/(B20+G20)</f>
+      <c r="J20" s="30">
+        <f>(D20+H20)/(B20+F20)</f>
         <v>0.32500000000000001</v>
       </c>
-      <c r="M20" s="16">
-        <f>(C20*D20)+(H20*I20)</f>
+      <c r="K20" s="31">
+        <f>(C20*D20)+(G20*H20)</f>
         <v>2550</v>
       </c>
-      <c r="N20" s="16">
-        <f>M20/(D20+I20)</f>
+      <c r="L20" s="31">
+        <f>K20/(D20+H20)</f>
         <v>196.15384615384616</v>
       </c>
-      <c r="O20" s="16">
+      <c r="M20" s="32">
         <f t="shared" si="2"/>
         <v>63.750000000000007</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A21" s="2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A21" s="23">
         <v>45676</v>
       </c>
-      <c r="B21">
-        <v>30</v>
-      </c>
-      <c r="C21" s="16">
-        <v>150</v>
-      </c>
-      <c r="D21">
-        <v>30</v>
-      </c>
-      <c r="E21" s="5">
+      <c r="B21" s="24">
+        <v>30</v>
+      </c>
+      <c r="C21" s="25">
+        <v>150</v>
+      </c>
+      <c r="D21" s="24">
+        <v>30</v>
+      </c>
+      <c r="E21" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G21">
-        <v>10</v>
-      </c>
-      <c r="H21" s="16">
-        <v>225</v>
-      </c>
-      <c r="I21">
+      <c r="F21" s="27">
+        <v>10</v>
+      </c>
+      <c r="G21" s="28">
+        <v>225</v>
+      </c>
+      <c r="H21" s="27">
         <v>9</v>
       </c>
-      <c r="J21" s="5">
+      <c r="I21" s="29">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="L21" s="5">
-        <f>(D21+I21)/(B21+G21)</f>
+      <c r="J21" s="30">
+        <f>(D21+H21)/(B21+F21)</f>
         <v>0.97499999999999998</v>
       </c>
-      <c r="M21" s="16">
-        <f>(C21*D21)+(H21*I21)</f>
+      <c r="K21" s="31">
+        <f>(C21*D21)+(G21*H21)</f>
         <v>6525</v>
       </c>
-      <c r="N21" s="16">
-        <f>M21/(D21+I21)</f>
+      <c r="L21" s="31">
+        <f>K21/(D21+H21)</f>
         <v>167.30769230769232</v>
       </c>
-      <c r="O21" s="16">
+      <c r="M21" s="32">
         <f t="shared" si="2"/>
         <v>163.125</v>
       </c>
     </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A22" s="2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" s="23">
         <v>45677</v>
       </c>
-      <c r="B22">
-        <v>30</v>
-      </c>
-      <c r="C22" s="16">
-        <v>150</v>
-      </c>
-      <c r="D22">
-        <v>30</v>
-      </c>
-      <c r="E22" s="5">
+      <c r="B22" s="24">
+        <v>30</v>
+      </c>
+      <c r="C22" s="25">
+        <v>150</v>
+      </c>
+      <c r="D22" s="24">
+        <v>30</v>
+      </c>
+      <c r="E22" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G22">
-        <v>10</v>
-      </c>
-      <c r="H22" s="16">
-        <v>225</v>
-      </c>
-      <c r="I22">
-        <v>10</v>
-      </c>
-      <c r="J22" s="5">
+      <c r="F22" s="27">
+        <v>10</v>
+      </c>
+      <c r="G22" s="28">
+        <v>225</v>
+      </c>
+      <c r="H22" s="27">
+        <v>10</v>
+      </c>
+      <c r="I22" s="29">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L22" s="5">
-        <f>(D22+I22)/(B22+G22)</f>
+      <c r="J22" s="30">
+        <f>(D22+H22)/(B22+F22)</f>
         <v>1</v>
       </c>
-      <c r="M22" s="16">
-        <f>(C22*D22)+(H22*I22)</f>
+      <c r="K22" s="31">
+        <f>(C22*D22)+(G22*H22)</f>
         <v>6750</v>
       </c>
-      <c r="N22" s="16">
-        <f>M22/(D22+I22)</f>
+      <c r="L22" s="31">
+        <f>K22/(D22+H22)</f>
         <v>168.75</v>
       </c>
-      <c r="O22" s="16">
+      <c r="M22" s="32">
         <f t="shared" si="2"/>
         <v>168.75</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A23" s="2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" s="23">
         <v>45678</v>
       </c>
-      <c r="B23">
-        <v>30</v>
-      </c>
-      <c r="C23" s="16">
-        <v>150</v>
-      </c>
-      <c r="D23">
+      <c r="B23" s="24">
+        <v>30</v>
+      </c>
+      <c r="C23" s="25">
+        <v>150</v>
+      </c>
+      <c r="D23" s="24">
         <v>15</v>
       </c>
-      <c r="E23" s="5">
+      <c r="E23" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G23">
-        <v>10</v>
-      </c>
-      <c r="H23" s="16">
-        <v>225</v>
-      </c>
-      <c r="I23">
+      <c r="F23" s="27">
+        <v>10</v>
+      </c>
+      <c r="G23" s="28">
+        <v>225</v>
+      </c>
+      <c r="H23" s="27">
         <v>2</v>
       </c>
-      <c r="J23" s="5">
+      <c r="I23" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L23" s="5">
-        <f>(D23+I23)/(B23+G23)</f>
+      <c r="J23" s="30">
+        <f>(D23+H23)/(B23+F23)</f>
         <v>0.42499999999999999</v>
       </c>
-      <c r="M23" s="16">
-        <f>(C23*D23)+(H23*I23)</f>
+      <c r="K23" s="31">
+        <f>(C23*D23)+(G23*H23)</f>
         <v>2700</v>
       </c>
-      <c r="N23" s="16">
-        <f>M23/(D23+I23)</f>
+      <c r="L23" s="31">
+        <f>K23/(D23+H23)</f>
         <v>158.8235294117647</v>
       </c>
-      <c r="O23" s="16">
+      <c r="M23" s="32">
         <f t="shared" si="2"/>
         <v>67.5</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A24" s="2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" s="23">
         <v>45679</v>
       </c>
-      <c r="B24">
-        <v>30</v>
-      </c>
-      <c r="C24" s="16">
-        <v>150</v>
-      </c>
-      <c r="D24">
-        <v>10</v>
-      </c>
-      <c r="E24" s="5">
+      <c r="B24" s="24">
+        <v>30</v>
+      </c>
+      <c r="C24" s="25">
+        <v>150</v>
+      </c>
+      <c r="D24" s="24">
+        <v>10</v>
+      </c>
+      <c r="E24" s="26">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G24">
-        <v>10</v>
-      </c>
-      <c r="H24" s="16">
-        <v>225</v>
-      </c>
-      <c r="I24">
+      <c r="F24" s="27">
+        <v>10</v>
+      </c>
+      <c r="G24" s="28">
+        <v>225</v>
+      </c>
+      <c r="H24" s="27">
         <v>4</v>
       </c>
-      <c r="J24" s="5">
+      <c r="I24" s="29">
         <f t="shared" si="1"/>
         <v>0.4</v>
       </c>
-      <c r="L24" s="5">
-        <f>(D24+I24)/(B24+G24)</f>
+      <c r="J24" s="30">
+        <f>(D24+H24)/(B24+F24)</f>
         <v>0.35</v>
       </c>
-      <c r="M24" s="16">
-        <f>(C24*D24)+(H24*I24)</f>
+      <c r="K24" s="31">
+        <f>(C24*D24)+(G24*H24)</f>
         <v>2400</v>
       </c>
-      <c r="N24" s="16">
-        <f>M24/(D24+I24)</f>
+      <c r="L24" s="31">
+        <f>K24/(D24+H24)</f>
         <v>171.42857142857142</v>
       </c>
-      <c r="O24" s="16">
+      <c r="M24" s="32">
         <f t="shared" si="2"/>
         <v>59.999999999999993</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A25" s="2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" s="23">
         <v>45680</v>
       </c>
-      <c r="B25">
-        <v>30</v>
-      </c>
-      <c r="C25" s="16">
-        <v>150</v>
-      </c>
-      <c r="D25">
+      <c r="B25" s="24">
+        <v>30</v>
+      </c>
+      <c r="C25" s="25">
+        <v>150</v>
+      </c>
+      <c r="D25" s="24">
         <v>15</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E25" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G25">
-        <v>10</v>
-      </c>
-      <c r="H25" s="16">
-        <v>225</v>
-      </c>
-      <c r="I25">
+      <c r="F25" s="27">
+        <v>10</v>
+      </c>
+      <c r="G25" s="28">
+        <v>225</v>
+      </c>
+      <c r="H25" s="27">
         <v>5</v>
       </c>
-      <c r="J25" s="5">
+      <c r="I25" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L25" s="5">
-        <f>(D25+I25)/(B25+G25)</f>
+      <c r="J25" s="30">
+        <f>(D25+H25)/(B25+F25)</f>
         <v>0.5</v>
       </c>
-      <c r="M25" s="16">
-        <f>(C25*D25)+(H25*I25)</f>
+      <c r="K25" s="31">
+        <f>(C25*D25)+(G25*H25)</f>
         <v>3375</v>
       </c>
-      <c r="N25" s="16">
-        <f>M25/(D25+I25)</f>
+      <c r="L25" s="31">
+        <f>K25/(D25+H25)</f>
         <v>168.75</v>
       </c>
-      <c r="O25" s="16">
+      <c r="M25" s="32">
         <f t="shared" si="2"/>
         <v>84.375</v>
       </c>
     </row>
-    <row r="26" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A26" s="2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" s="23">
         <v>45681</v>
       </c>
-      <c r="B26">
-        <v>30</v>
-      </c>
-      <c r="C26" s="16">
-        <v>150</v>
-      </c>
-      <c r="D26">
+      <c r="B26" s="24">
+        <v>30</v>
+      </c>
+      <c r="C26" s="25">
+        <v>150</v>
+      </c>
+      <c r="D26" s="24">
         <v>21</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E26" s="26">
         <f t="shared" si="0"/>
         <v>0.7</v>
       </c>
-      <c r="G26">
-        <v>10</v>
-      </c>
-      <c r="H26" s="16">
-        <v>225</v>
-      </c>
-      <c r="I26">
+      <c r="F26" s="27">
+        <v>10</v>
+      </c>
+      <c r="G26" s="28">
+        <v>225</v>
+      </c>
+      <c r="H26" s="27">
         <v>5</v>
       </c>
-      <c r="J26" s="5">
+      <c r="I26" s="29">
         <f t="shared" si="1"/>
         <v>0.5</v>
       </c>
-      <c r="L26" s="5">
-        <f>(D26+I26)/(B26+G26)</f>
+      <c r="J26" s="30">
+        <f>(D26+H26)/(B26+F26)</f>
         <v>0.65</v>
       </c>
-      <c r="M26" s="16">
-        <f>(C26*D26)+(H26*I26)</f>
+      <c r="K26" s="31">
+        <f>(C26*D26)+(G26*H26)</f>
         <v>4275</v>
       </c>
-      <c r="N26" s="16">
-        <f>M26/(D26+I26)</f>
+      <c r="L26" s="31">
+        <f>K26/(D26+H26)</f>
         <v>164.42307692307693</v>
       </c>
-      <c r="O26" s="16">
+      <c r="M26" s="32">
         <f t="shared" si="2"/>
         <v>106.87500000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A27" s="2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" s="23">
         <v>45682</v>
       </c>
-      <c r="B27">
-        <v>30</v>
-      </c>
-      <c r="C27" s="16">
-        <v>150</v>
-      </c>
-      <c r="D27">
+      <c r="B27" s="24">
+        <v>30</v>
+      </c>
+      <c r="C27" s="25">
+        <v>150</v>
+      </c>
+      <c r="D27" s="24">
         <v>5</v>
       </c>
-      <c r="E27" s="5">
+      <c r="E27" s="26">
         <f t="shared" si="0"/>
         <v>0.16666666666666666</v>
       </c>
-      <c r="G27">
-        <v>10</v>
-      </c>
-      <c r="H27" s="16">
-        <v>225</v>
-      </c>
-      <c r="I27">
+      <c r="F27" s="27">
+        <v>10</v>
+      </c>
+      <c r="G27" s="28">
+        <v>225</v>
+      </c>
+      <c r="H27" s="27">
         <v>2</v>
       </c>
-      <c r="J27" s="5">
+      <c r="I27" s="29">
         <f t="shared" si="1"/>
         <v>0.2</v>
       </c>
-      <c r="L27" s="5">
-        <f>(D27+I27)/(B27+G27)</f>
+      <c r="J27" s="30">
+        <f>(D27+H27)/(B27+F27)</f>
         <v>0.17499999999999999</v>
       </c>
-      <c r="M27" s="16">
-        <f>(C27*D27)+(H27*I27)</f>
+      <c r="K27" s="31">
+        <f>(C27*D27)+(G27*H27)</f>
         <v>1200</v>
       </c>
-      <c r="N27" s="16">
-        <f>M27/(D27+I27)</f>
+      <c r="L27" s="31">
+        <f>K27/(D27+H27)</f>
         <v>171.42857142857142</v>
       </c>
-      <c r="O27" s="16">
+      <c r="M27" s="32">
         <f t="shared" si="2"/>
         <v>29.999999999999996</v>
       </c>
     </row>
-    <row r="28" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A28" s="2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" s="23">
         <v>45683</v>
       </c>
-      <c r="B28">
-        <v>30</v>
-      </c>
-      <c r="C28" s="16">
-        <v>150</v>
-      </c>
-      <c r="D28">
-        <v>30</v>
-      </c>
-      <c r="E28" s="5">
+      <c r="B28" s="24">
+        <v>30</v>
+      </c>
+      <c r="C28" s="25">
+        <v>150</v>
+      </c>
+      <c r="D28" s="24">
+        <v>30</v>
+      </c>
+      <c r="E28" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G28">
-        <v>10</v>
-      </c>
-      <c r="H28" s="16">
-        <v>225</v>
-      </c>
-      <c r="I28">
+      <c r="F28" s="27">
+        <v>10</v>
+      </c>
+      <c r="G28" s="28">
+        <v>225</v>
+      </c>
+      <c r="H28" s="27">
         <v>0</v>
       </c>
-      <c r="J28" s="5">
+      <c r="I28" s="29">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L28" s="5">
-        <f>(D28+I28)/(B28+G28)</f>
+      <c r="J28" s="30">
+        <f>(D28+H28)/(B28+F28)</f>
         <v>0.75</v>
       </c>
-      <c r="M28" s="16">
-        <f>(C28*D28)+(H28*I28)</f>
+      <c r="K28" s="31">
+        <f>(C28*D28)+(G28*H28)</f>
         <v>4500</v>
       </c>
-      <c r="N28" s="16">
-        <f>M28/(D28+I28)</f>
-        <v>150</v>
-      </c>
-      <c r="O28" s="16">
+      <c r="L28" s="31">
+        <f>K28/(D28+H28)</f>
+        <v>150</v>
+      </c>
+      <c r="M28" s="32">
         <f t="shared" si="2"/>
         <v>112.5</v>
       </c>
     </row>
-    <row r="29" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A29" s="2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" s="23">
         <v>45684</v>
       </c>
-      <c r="B29">
-        <v>30</v>
-      </c>
-      <c r="C29" s="16">
-        <v>150</v>
-      </c>
-      <c r="D29">
-        <v>30</v>
-      </c>
-      <c r="E29" s="5">
+      <c r="B29" s="24">
+        <v>30</v>
+      </c>
+      <c r="C29" s="25">
+        <v>150</v>
+      </c>
+      <c r="D29" s="24">
+        <v>30</v>
+      </c>
+      <c r="E29" s="26">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
-      <c r="G29">
-        <v>10</v>
-      </c>
-      <c r="H29" s="16">
-        <v>225</v>
-      </c>
-      <c r="I29">
+      <c r="F29" s="27">
+        <v>10</v>
+      </c>
+      <c r="G29" s="28">
+        <v>225</v>
+      </c>
+      <c r="H29" s="27">
         <v>3</v>
       </c>
-      <c r="J29" s="5">
+      <c r="I29" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L29" s="5">
-        <f>(D29+I29)/(B29+G29)</f>
+      <c r="J29" s="30">
+        <f>(D29+H29)/(B29+F29)</f>
         <v>0.82499999999999996</v>
       </c>
-      <c r="M29" s="16">
-        <f>(C29*D29)+(H29*I29)</f>
+      <c r="K29" s="31">
+        <f>(C29*D29)+(G29*H29)</f>
         <v>5175</v>
       </c>
-      <c r="N29" s="16">
-        <f>M29/(D29+I29)</f>
+      <c r="L29" s="31">
+        <f>K29/(D29+H29)</f>
         <v>156.81818181818181</v>
       </c>
-      <c r="O29" s="16">
+      <c r="M29" s="32">
         <f t="shared" si="2"/>
         <v>129.375</v>
       </c>
     </row>
-    <row r="30" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A30" s="2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" s="23">
         <v>45685</v>
       </c>
-      <c r="B30">
-        <v>30</v>
-      </c>
-      <c r="C30" s="16">
-        <v>150</v>
-      </c>
-      <c r="D30">
+      <c r="B30" s="24">
+        <v>30</v>
+      </c>
+      <c r="C30" s="25">
+        <v>150</v>
+      </c>
+      <c r="D30" s="24">
         <v>15</v>
       </c>
-      <c r="E30" s="5">
+      <c r="E30" s="26">
         <f t="shared" si="0"/>
         <v>0.5</v>
       </c>
-      <c r="G30">
-        <v>10</v>
-      </c>
-      <c r="H30" s="16">
-        <v>225</v>
-      </c>
-      <c r="I30">
+      <c r="F30" s="27">
+        <v>10</v>
+      </c>
+      <c r="G30" s="28">
+        <v>225</v>
+      </c>
+      <c r="H30" s="27">
         <v>3</v>
       </c>
-      <c r="J30" s="5">
+      <c r="I30" s="29">
         <f t="shared" si="1"/>
         <v>0.3</v>
       </c>
-      <c r="L30" s="5">
-        <f>(D30+I30)/(B30+G30)</f>
+      <c r="J30" s="30">
+        <f>(D30+H30)/(B30+F30)</f>
         <v>0.45</v>
       </c>
-      <c r="M30" s="16">
-        <f>(C30*D30)+(H30*I30)</f>
+      <c r="K30" s="31">
+        <f>(C30*D30)+(G30*H30)</f>
         <v>2925</v>
       </c>
-      <c r="N30" s="16">
-        <f>M30/(D30+I30)</f>
+      <c r="L30" s="31">
+        <f>K30/(D30+H30)</f>
         <v>162.5</v>
       </c>
-      <c r="O30" s="16">
+      <c r="M30" s="32">
         <f t="shared" si="2"/>
         <v>73.125</v>
       </c>
     </row>
-    <row r="31" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A31" s="2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" s="23">
         <v>45686</v>
       </c>
-      <c r="B31">
-        <v>30</v>
-      </c>
-      <c r="C31" s="16">
-        <v>150</v>
-      </c>
-      <c r="D31">
+      <c r="B31" s="24">
+        <v>30</v>
+      </c>
+      <c r="C31" s="25">
+        <v>150</v>
+      </c>
+      <c r="D31" s="24">
         <v>17</v>
       </c>
-      <c r="E31" s="5">
+      <c r="E31" s="26">
         <f t="shared" si="0"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="G31">
-        <v>10</v>
-      </c>
-      <c r="H31" s="16">
-        <v>225</v>
-      </c>
-      <c r="I31">
+      <c r="F31" s="27">
+        <v>10</v>
+      </c>
+      <c r="G31" s="28">
+        <v>225</v>
+      </c>
+      <c r="H31" s="27">
         <v>8</v>
       </c>
-      <c r="J31" s="5">
+      <c r="I31" s="29">
         <f t="shared" si="1"/>
         <v>0.8</v>
       </c>
-      <c r="L31" s="5">
-        <f>(D31+I31)/(B31+G31)</f>
+      <c r="J31" s="30">
+        <f>(D31+H31)/(B31+F31)</f>
         <v>0.625</v>
       </c>
-      <c r="M31" s="16">
-        <f>(C31*D31)+(H31*I31)</f>
+      <c r="K31" s="31">
+        <f>(C31*D31)+(G31*H31)</f>
         <v>4350</v>
       </c>
-      <c r="N31" s="16">
-        <f>M31/(D31+I31)</f>
+      <c r="L31" s="31">
+        <f>K31/(D31+H31)</f>
         <v>174</v>
       </c>
-      <c r="O31" s="16">
+      <c r="M31" s="32">
         <f t="shared" si="2"/>
         <v>108.75</v>
       </c>
     </row>
-    <row r="32" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A32" s="2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" s="23">
         <v>45687</v>
       </c>
-      <c r="B32">
-        <v>30</v>
-      </c>
-      <c r="C32" s="16">
-        <v>150</v>
-      </c>
-      <c r="D32">
+      <c r="B32" s="24">
+        <v>30</v>
+      </c>
+      <c r="C32" s="25">
+        <v>150</v>
+      </c>
+      <c r="D32" s="24">
         <v>17</v>
       </c>
-      <c r="E32" s="5">
+      <c r="E32" s="26">
         <f t="shared" si="0"/>
         <v>0.56666666666666665</v>
       </c>
-      <c r="G32">
-        <v>10</v>
-      </c>
-      <c r="H32" s="16">
-        <v>225</v>
-      </c>
-      <c r="I32">
+      <c r="F32" s="27">
+        <v>10</v>
+      </c>
+      <c r="G32" s="28">
+        <v>225</v>
+      </c>
+      <c r="H32" s="27">
         <v>9</v>
       </c>
-      <c r="J32" s="5">
+      <c r="I32" s="29">
         <f t="shared" si="1"/>
         <v>0.9</v>
       </c>
-      <c r="L32" s="5">
-        <f>(D32+I32)/(B32+G32)</f>
+      <c r="J32" s="30">
+        <f>(D32+H32)/(B32+F32)</f>
         <v>0.65</v>
       </c>
-      <c r="M32" s="16">
-        <f>(C32*D32)+(H32*I32)</f>
+      <c r="K32" s="31">
+        <f>(C32*D32)+(G32*H32)</f>
         <v>4575</v>
       </c>
-      <c r="N32" s="16">
-        <f>M32/(D32+I32)</f>
+      <c r="L32" s="31">
+        <f>K32/(D32+H32)</f>
         <v>175.96153846153845</v>
       </c>
-      <c r="O32" s="16">
+      <c r="M32" s="32">
         <f t="shared" si="2"/>
         <v>114.375</v>
       </c>
     </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A33" s="2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A33" s="33">
         <v>45688</v>
       </c>
-      <c r="B33">
-        <v>30</v>
-      </c>
-      <c r="C33" s="16">
-        <v>150</v>
-      </c>
-      <c r="D33">
+      <c r="B33" s="34">
+        <v>30</v>
+      </c>
+      <c r="C33" s="35">
+        <v>150</v>
+      </c>
+      <c r="D33" s="34">
         <v>29</v>
       </c>
-      <c r="E33" s="5">
+      <c r="E33" s="36">
         <f t="shared" si="0"/>
         <v>0.96666666666666667</v>
       </c>
-      <c r="G33">
-        <v>10</v>
-      </c>
-      <c r="H33" s="16">
-        <v>225</v>
-      </c>
-      <c r="I33">
-        <v>10</v>
-      </c>
-      <c r="J33" s="5">
+      <c r="F33" s="37">
+        <v>10</v>
+      </c>
+      <c r="G33" s="38">
+        <v>225</v>
+      </c>
+      <c r="H33" s="37">
+        <v>10</v>
+      </c>
+      <c r="I33" s="39">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="L33" s="5">
-        <f>(D33+I33)/(B33+G33)</f>
+      <c r="J33" s="40">
+        <f>(D33+H33)/(B33+F33)</f>
         <v>0.97499999999999998</v>
       </c>
-      <c r="M33" s="16">
-        <f>(C33*D33)+(H33*I33)</f>
+      <c r="K33" s="41">
+        <f>(C33*D33)+(G33*H33)</f>
         <v>6600</v>
       </c>
-      <c r="N33" s="16">
-        <f>M33/(D33+I33)</f>
+      <c r="L33" s="41">
+        <f>K33/(D33+H33)</f>
         <v>169.23076923076923</v>
       </c>
-      <c r="O33" s="16">
+      <c r="M33" s="42">
         <f t="shared" si="2"/>
         <v>165</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
-    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="B1:E1"/>
-    <mergeCell ref="G1:J1"/>
+    <mergeCell ref="F1:I1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>